<commit_message>
add company schema and interceptor logice
</commit_message>
<xml_diff>
--- a/seeds/schemas/accounts.xlsx
+++ b/seeds/schemas/accounts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="columns_mapper" sheetId="1" state="visible" r:id="rId3"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="106">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -91,7 +91,7 @@
     <t xml:space="preserve">moderator role</t>
   </si>
   <si>
-    <t xml:space="preserve">BucketCreate|BucketUpdate|SettingList|RoleList</t>
+    <t xml:space="preserve">CompanyCreate|CompanyFind|CompanyList|CompanyUpdate|PageCreate|PageFind|PageList|PageUpdate|SectionCreate|SectionFind|SectionList|SectionUpdate</t>
   </si>
   <si>
     <t xml:space="preserve">navigation_bar_name</t>
@@ -100,6 +100,12 @@
     <t xml:space="preserve">admins backoffice</t>
   </si>
   <si>
+    <t xml:space="preserve">admin backoffice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">company backoffice</t>
+  </si>
+  <si>
     <t xml:space="preserve">menu_key</t>
   </si>
   <si>
@@ -325,7 +331,7 @@
     <t xml:space="preserve">user_password#</t>
   </si>
   <si>
-    <t xml:space="preserve">karim</t>
+    <t xml:space="preserve">ahmed</t>
   </si>
   <si>
     <t xml:space="preserve">admin</t>
@@ -334,19 +340,16 @@
     <t xml:space="preserve">0 1118614244</t>
   </si>
   <si>
-    <t xml:space="preserve">karim@devkit.com</t>
+    <t xml:space="preserve">ahme@devkit.com</t>
   </si>
   <si>
     <t xml:space="preserve">super admin</t>
   </si>
   <si>
-    <t xml:space="preserve">yossuf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">company</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yossuf@devkit.com</t>
+    <t xml:space="preserve">kareem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kareem@devkit.com</t>
   </si>
 </sst>
 </file>
@@ -739,7 +742,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -820,10 +823,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D1048576"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5078125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -832,6 +835,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="94.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="42.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -862,8 +866,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C3" s="5"/>
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="5"/>
@@ -901,19 +908,6 @@
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="5"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="5"/>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -933,29 +927,39 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="40.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.81"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
         <v>20</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
         <v>21</v>
       </c>
+      <c r="B2" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7"/>
+      <c r="B3" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7"/>
@@ -1005,7 +1009,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1019,19 +1023,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>4</v>
@@ -1039,19 +1043,19 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>21</v>
@@ -1059,16 +1063,16 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="7" t="s">
@@ -1077,16 +1081,16 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="7" t="s">
@@ -1130,19 +1134,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>6</v>
@@ -1156,25 +1160,25 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>21</v>
@@ -1182,25 +1186,25 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H3" s="7" t="s">
         <v>21</v>
@@ -1208,25 +1212,25 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>21</v>
@@ -1234,25 +1238,25 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>21</v>
@@ -1260,25 +1264,25 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>21</v>
@@ -1286,25 +1290,25 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>21</v>
@@ -1312,25 +1316,25 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="H8" s="7" t="s">
         <v>21</v>
@@ -1338,25 +1342,25 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>21</v>
@@ -1400,19 +1404,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>6</v>
@@ -1426,25 +1430,25 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>46</v>
-      </c>
       <c r="G2" s="7" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>21</v>
@@ -1470,8 +1474,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1486,19 +1490,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>10</v>
@@ -1506,36 +1510,36 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E2" s="8" t="n">
         <v>123456</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C3" s="4" t="n">
         <v>1202290100</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E3" s="8" t="n">
         <v>123456</v>
@@ -1543,12 +1547,15 @@
       <c r="F3" s="9" t="s">
         <v>17</v>
       </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F5" s="9"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="karim@devkit.com"/>
-    <hyperlink ref="D3" r:id="rId2" display="yossuf@devkit.com"/>
+    <hyperlink ref="D2" r:id="rId1" display="ahme@devkit.com"/>
+    <hyperlink ref="D3" r:id="rId2" display="kareem@devkit.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
rename company to be tenant and add the tenant checks on the interceptor and get the tenant id from context at the repo layer
</commit_message>
<xml_diff>
--- a/seeds/schemas/accounts.xlsx
+++ b/seeds/schemas/accounts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="columns_mapper" sheetId="1" state="visible" r:id="rId3"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="105">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -91,16 +91,13 @@
     <t xml:space="preserve">moderator role</t>
   </si>
   <si>
-    <t xml:space="preserve">CompanyCreate|CompanyFind|CompanyList|CompanyUpdate|PageCreate|PageFind|PageList|PageUpdate|SectionCreate|SectionFind|SectionList|SectionUpdate</t>
+    <t xml:space="preserve">TenantCreate|TenantFind|TenantList|TenantUpdate|PageCreate|PageFind|PageList|PageUpdate|SectionCreate|SectionFind|SectionList|SectionUpdate</t>
   </si>
   <si>
     <t xml:space="preserve">navigation_bar_name</t>
   </si>
   <si>
     <t xml:space="preserve">admins backoffice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">admin backoffice</t>
   </si>
   <si>
     <t xml:space="preserve">company backoffice</t>
@@ -825,8 +822,8 @@
   </sheetPr>
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5078125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -852,7 +849,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="16.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
         <v>17</v>
       </c>
@@ -929,8 +926,8 @@
   </sheetPr>
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E31" activeCellId="0" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -952,13 +949,13 @@
         <v>21</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7"/>
       <c r="B3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1009,7 +1006,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1023,19 +1020,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>27</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>28</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>4</v>
@@ -1043,19 +1040,19 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>32</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>33</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>21</v>
@@ -1063,16 +1060,16 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="C3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="7" t="s">
         <v>36</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>37</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="7" t="s">
@@ -1081,16 +1078,16 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="C4" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="7" t="s">
         <v>40</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>41</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="7" t="s">
@@ -1117,8 +1114,8 @@
   </sheetPr>
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1134,19 +1131,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>27</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>28</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>6</v>
@@ -1160,25 +1157,25 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="F2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>46</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>47</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>21</v>
@@ -1186,25 +1183,25 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="C3" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="E3" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="F3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>52</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>53</v>
       </c>
       <c r="H3" s="7" t="s">
         <v>21</v>
@@ -1212,25 +1209,25 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="C4" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="E4" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="F4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>58</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>59</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>21</v>
@@ -1238,25 +1235,25 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="C5" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="E5" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="F5" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>64</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>65</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>21</v>
@@ -1264,25 +1261,25 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="E6" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="F6" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>70</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>71</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>21</v>
@@ -1290,25 +1287,25 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="C7" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="E7" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="F7" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>76</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>77</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>21</v>
@@ -1316,25 +1313,25 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="C8" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="E8" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="F8" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" s="7" t="s">
         <v>82</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>83</v>
       </c>
       <c r="H8" s="7" t="s">
         <v>21</v>
@@ -1342,25 +1339,25 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="C9" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="E9" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="F9" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" s="7" t="s">
         <v>88</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>89</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>21</v>
@@ -1386,8 +1383,8 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H47" activeCellId="0" sqref="H47"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1404,19 +1401,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>27</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>28</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>6</v>
@@ -1430,25 +1427,25 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="E2" s="7" t="s">
+      <c r="F2" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>92</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>93</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>21</v>
@@ -1474,7 +1471,7 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -1490,19 +1487,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>98</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>10</v>
@@ -1510,36 +1507,36 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>101</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>102</v>
       </c>
       <c r="E2" s="8" t="n">
         <v>123456</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C3" s="4" t="n">
         <v>1202290100</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E3" s="8" t="n">
         <v>123456</v>

</xml_diff>

<commit_message>
add icon find endpoint
</commit_message>
<xml_diff>
--- a/seeds/schemas/accounts.xlsx
+++ b/seeds/schemas/accounts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="columns_mapper" sheetId="1" state="visible" r:id="rId3"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="228">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -88,12 +88,378 @@
     <t xml:space="preserve">moderator</t>
   </si>
   <si>
-    <t xml:space="preserve">moderator role</t>
+    <t xml:space="preserve">moderator role1</t>
   </si>
   <si>
     <t xml:space="preserve">TenantCreate|TenantFind|TenantList|TenantUpdate|PageCreate|PageFind|PageList|PageUpdate|SectionCreate|SectionFind|SectionList|SectionUpdate</t>
   </si>
   <si>
+    <t xml:space="preserve">moderator2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator62</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator role62</t>
+  </si>
+  <si>
     <t xml:space="preserve">navigation_bar_name</t>
   </si>
   <si>
@@ -127,7 +493,7 @@
     <t xml:space="preserve">لوحة التحكم</t>
   </si>
   <si>
-    <t xml:space="preserve">dashboard_icon</t>
+    <t xml:space="preserve">dashboard</t>
   </si>
   <si>
     <t xml:space="preserve">/dashboard</t>
@@ -142,7 +508,7 @@
     <t xml:space="preserve">الحسابات</t>
   </si>
   <si>
-    <t xml:space="preserve">accounts_icon</t>
+    <t xml:space="preserve">people</t>
   </si>
   <si>
     <t xml:space="preserve">03_system</t>
@@ -154,7 +520,7 @@
     <t xml:space="preserve">النظام</t>
   </si>
   <si>
-    <t xml:space="preserve">system_icon</t>
+    <t xml:space="preserve">settings</t>
   </si>
   <si>
     <t xml:space="preserve">01_roles</t>
@@ -166,10 +532,10 @@
     <t xml:space="preserve">الأدوار</t>
   </si>
   <si>
-    <t xml:space="preserve">roles_icon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/accounts/roles</t>
+    <t xml:space="preserve">group_users</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/accounts/role</t>
   </si>
   <si>
     <t xml:space="preserve">RoleList</t>
@@ -184,10 +550,10 @@
     <t xml:space="preserve">المستخدمين</t>
   </si>
   <si>
-    <t xml:space="preserve">users_icon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/accounts/users</t>
+    <t xml:space="preserve">user_add</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/accounts/user</t>
   </si>
   <si>
     <t xml:space="preserve">UserList</t>
@@ -202,7 +568,7 @@
     <t xml:space="preserve">القوائم</t>
   </si>
   <si>
-    <t xml:space="preserve">navigation_icon</t>
+    <t xml:space="preserve">maps</t>
   </si>
   <si>
     <t xml:space="preserve">/accounts/navigation</t>
@@ -220,10 +586,10 @@
     <t xml:space="preserve">الترجمات</t>
   </si>
   <si>
-    <t xml:space="preserve">translations_icon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/system/translations</t>
+    <t xml:space="preserve">globe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/system/translation</t>
   </si>
   <si>
     <t xml:space="preserve">TranslationList</t>
@@ -238,10 +604,10 @@
     <t xml:space="preserve">الأيقونات</t>
   </si>
   <si>
-    <t xml:space="preserve">icons_icon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/system/icons</t>
+    <t xml:space="preserve">design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/system/icon</t>
   </si>
   <si>
     <t xml:space="preserve">IconList</t>
@@ -256,10 +622,10 @@
     <t xml:space="preserve">المجلدات</t>
   </si>
   <si>
-    <t xml:space="preserve">buckets_icon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/system/buckets</t>
+    <t xml:space="preserve">folder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/system/bucket</t>
   </si>
   <si>
     <t xml:space="preserve">BucketList</t>
@@ -274,10 +640,10 @@
     <t xml:space="preserve">الملفات</t>
   </si>
   <si>
-    <t xml:space="preserve">objects_icon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/system/objects</t>
+    <t xml:space="preserve">file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/system/object</t>
   </si>
   <si>
     <t xml:space="preserve">ObjectList</t>
@@ -295,7 +661,7 @@
     <t xml:space="preserve">settings_icon</t>
   </si>
   <si>
-    <t xml:space="preserve">/system/settings</t>
+    <t xml:space="preserve">/system/setting</t>
   </si>
   <si>
     <t xml:space="preserve">SettingList</t>
@@ -305,6 +671,9 @@
   </si>
   <si>
     <t xml:space="preserve">Users Create</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user_verified</t>
   </si>
   <si>
     <t xml:space="preserve">/accounts/users/create</t>
@@ -356,7 +725,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -390,6 +759,13 @@
       <sz val="12"/>
       <name val="Times New Roman"/>
       <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="DejaVu Serif"/>
+      <family val="1"/>
       <charset val="1"/>
     </font>
     <font>
@@ -454,7 +830,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -487,11 +863,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -820,10 +1200,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5078125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -863,47 +1243,859 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="5"/>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="5"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="5"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="5"/>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="5"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="5"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="5"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="5"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="5"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="5"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="5"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="5"/>
+    <row r="3" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D30" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D31" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D34" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D35" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D36" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D37" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D38" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D39" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D40" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D41" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D42" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D43" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D44" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D45" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D46" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D47" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D48" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D49" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D50" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D51" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D52" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D53" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D54" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D55" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D56" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D57" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D58" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D59" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D60" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D61" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D62" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D63" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -926,7 +2118,7 @@
   </sheetPr>
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E31" activeCellId="0" sqref="E31"/>
     </sheetView>
   </sheetViews>
@@ -938,24 +2130,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>20</v>
+        <v>142</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>21</v>
+        <v>143</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>21</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7"/>
       <c r="B3" s="1" t="s">
-        <v>22</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1006,7 +2198,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1020,19 +2212,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>23</v>
+        <v>145</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>24</v>
+        <v>146</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>25</v>
+        <v>147</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>26</v>
+        <v>148</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>27</v>
+        <v>149</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>4</v>
@@ -1040,58 +2232,58 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>28</v>
+        <v>150</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>29</v>
+        <v>151</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>31</v>
+        <v>152</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>153</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>32</v>
+        <v>154</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>21</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>33</v>
+        <v>155</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>34</v>
+        <v>156</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>36</v>
+        <v>157</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>158</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="7" t="s">
-        <v>21</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>37</v>
+        <v>159</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>38</v>
+        <v>160</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>40</v>
+        <v>161</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>162</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="7" t="s">
-        <v>21</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -1115,7 +2307,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1131,19 +2323,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>23</v>
+        <v>145</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>24</v>
+        <v>146</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>25</v>
+        <v>147</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>26</v>
+        <v>148</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>27</v>
+        <v>149</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>6</v>
@@ -1157,210 +2349,210 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>41</v>
+        <v>163</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>42</v>
+        <v>164</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>43</v>
+        <v>165</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>44</v>
+        <v>166</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>45</v>
+        <v>167</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>33</v>
+        <v>155</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>46</v>
+        <v>168</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>21</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>47</v>
+        <v>169</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>48</v>
+        <v>170</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>50</v>
+        <v>171</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>172</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>51</v>
+        <v>173</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>33</v>
+        <v>155</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>52</v>
+        <v>174</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>21</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>53</v>
+        <v>175</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>54</v>
+        <v>176</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>56</v>
+        <v>177</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>178</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>57</v>
+        <v>179</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>33</v>
+        <v>155</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>58</v>
+        <v>180</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>21</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>59</v>
+        <v>181</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>60</v>
+        <v>182</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>62</v>
+        <v>183</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>184</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>63</v>
+        <v>185</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>37</v>
+        <v>159</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>64</v>
+        <v>186</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>21</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>65</v>
+        <v>187</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>66</v>
+        <v>188</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>68</v>
+        <v>189</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>190</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>69</v>
+        <v>191</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>37</v>
+        <v>159</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>70</v>
+        <v>192</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>21</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
-        <v>71</v>
+        <v>193</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>72</v>
+        <v>194</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>73</v>
+        <v>195</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>74</v>
+        <v>196</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>75</v>
+        <v>197</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>37</v>
+        <v>159</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>76</v>
+        <v>198</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>21</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>77</v>
+        <v>199</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>78</v>
+        <v>200</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>79</v>
+        <v>201</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>80</v>
+        <v>202</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>81</v>
+        <v>203</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>37</v>
+        <v>159</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>82</v>
+        <v>204</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>21</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
-        <v>83</v>
+        <v>205</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>84</v>
+        <v>206</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>85</v>
+        <v>207</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>86</v>
+        <v>208</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>87</v>
+        <v>209</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>37</v>
+        <v>159</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>88</v>
+        <v>210</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>21</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -1384,7 +2576,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1401,19 +2593,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>23</v>
+        <v>145</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>24</v>
+        <v>146</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>25</v>
+        <v>147</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>26</v>
+        <v>148</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>27</v>
+        <v>149</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>6</v>
@@ -1427,28 +2619,28 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>89</v>
+        <v>211</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>90</v>
+        <v>212</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>50</v>
+        <v>171</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>213</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>91</v>
+        <v>214</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>47</v>
+        <v>169</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>92</v>
+        <v>215</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>21</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -1487,19 +2679,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>93</v>
+        <v>216</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>94</v>
+        <v>217</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>95</v>
+        <v>218</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>96</v>
+        <v>219</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>97</v>
+        <v>220</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>10</v>
@@ -1507,46 +2699,46 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>98</v>
+        <v>221</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>99</v>
+        <v>222</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>100</v>
+        <v>223</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="E2" s="8" t="n">
+        <v>224</v>
+      </c>
+      <c r="E2" s="9" t="n">
         <v>123456</v>
       </c>
-      <c r="F2" s="9" t="s">
-        <v>102</v>
+      <c r="F2" s="10" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>103</v>
+        <v>226</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>99</v>
+        <v>222</v>
       </c>
       <c r="C3" s="4" t="n">
         <v>1202290100</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="E3" s="8" t="n">
+        <v>227</v>
+      </c>
+      <c r="E3" s="9" t="n">
         <v>123456</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="10" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F5" s="9"/>
+      <c r="F5" s="10"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>

<commit_message>
sync with abc webiste data
</commit_message>
<xml_diff>
--- a/seeds/schemas/accounts.xlsx
+++ b/seeds/schemas/accounts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="columns_mapper" sheetId="1" state="visible" r:id="rId3"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="127">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -157,6 +157,18 @@
     <t xml:space="preserve">settings</t>
   </si>
   <si>
+    <t xml:space="preserve">01_tn_dashboard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02_tn_tenants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Companies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">الشركات</t>
+  </si>
+  <si>
     <t xml:space="preserve">01_roles</t>
   </si>
   <si>
@@ -296,6 +308,60 @@
   </si>
   <si>
     <t xml:space="preserve">SettingList</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01_tn_tenants_tenants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/tenants/tenant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TenantList</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02_tn_tenants_sections</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sections</t>
+  </si>
+  <si>
+    <t xml:space="preserve">الاقسام</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/tenants/section</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SectionList</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03_tn_tenants_pages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">الصفحات</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/tenants/page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PageList</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04_tn_tenants_partials</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Partials</t>
+  </si>
+  <si>
+    <t xml:space="preserve">الخدمات و المشاريع</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/tenants/partial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PartialList</t>
   </si>
   <si>
     <t xml:space="preserve">02_users_create</t>
@@ -356,7 +422,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -398,6 +464,12 @@
       <name val="DejaVu Serif"/>
       <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="CommitMono Nerd Font"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="12"/>
@@ -461,7 +533,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -498,11 +570,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -750,7 +826,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -834,7 +910,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5078125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -860,7 +936,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
         <v>17</v>
       </c>
@@ -896,7 +972,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E31" activeCellId="0" sqref="E31"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -972,19 +1048,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="2" width="12.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="15.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="20.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="19.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="67.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="14.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="9.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="10.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="9.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="10.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="16.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1062,6 +1139,51 @@
       <c r="F4" s="7" t="s">
         <v>21</v>
       </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="7"/>
+      <c r="F6" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:E4"/>
@@ -1081,10 +1203,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1126,25 +1248,25 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>33</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>21</v>
@@ -1152,19 +1274,19 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>33</v>
@@ -1178,25 +1300,25 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>33</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>21</v>
@@ -1204,25 +1326,25 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>37</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>21</v>
@@ -1230,25 +1352,25 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>37</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>21</v>
@@ -1256,25 +1378,25 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>37</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>21</v>
@@ -1282,25 +1404,25 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>37</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="H8" s="7" t="s">
         <v>21</v>
@@ -1308,28 +1430,132 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>37</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1353,7 +1579,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
+      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1396,25 +1622,25 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>88</v>
+        <v>110</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>90</v>
+        <v>112</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>92</v>
+        <v>114</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>21</v>
@@ -1440,8 +1666,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1456,19 +1682,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>93</v>
+        <v>115</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>95</v>
+        <v>117</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>96</v>
+        <v>118</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>97</v>
+        <v>119</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>10</v>
@@ -1476,46 +1702,46 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>98</v>
+        <v>120</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>99</v>
+        <v>121</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>100</v>
+        <v>122</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="E2" s="9" t="n">
+        <v>123</v>
+      </c>
+      <c r="E2" s="10" t="n">
         <v>12345678</v>
       </c>
-      <c r="F2" s="10" t="s">
-        <v>102</v>
+      <c r="F2" s="11" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>103</v>
+        <v>125</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>99</v>
+        <v>121</v>
       </c>
       <c r="C3" s="4" t="n">
         <v>1202290100</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="E3" s="9" t="n">
+        <v>126</v>
+      </c>
+      <c r="E3" s="10" t="n">
         <v>12345678</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="11" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F5" s="10"/>
+      <c r="F5" s="11"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>

<commit_message>
work on auth sessions
</commit_message>
<xml_diff>
--- a/seeds/schemas/accounts.xlsx
+++ b/seeds/schemas/accounts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="columns_mapper" sheetId="1" state="visible" r:id="rId3"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="176">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -285,7 +285,7 @@
     <t xml:space="preserve">timer-2-line</t>
   </si>
   <si>
-    <t xml:space="preserve">/accounts/sessions</t>
+    <t xml:space="preserve">/accounts/session</t>
   </si>
   <si>
     <t xml:space="preserve">AuthSessionList</t>
@@ -303,7 +303,7 @@
     <t xml:space="preserve">الأيقونات</t>
   </si>
   <si>
-    <t xml:space="preserve">/public/icons</t>
+    <t xml:space="preserve">/public/icon</t>
   </si>
   <si>
     <t xml:space="preserve">IconList</t>
@@ -324,7 +324,7 @@
     <t xml:space="preserve">safe-line</t>
   </si>
   <si>
-    <t xml:space="preserve">/public/buckets</t>
+    <t xml:space="preserve">/public/bucket</t>
   </si>
   <si>
     <t xml:space="preserve">BucketList</t>
@@ -342,7 +342,7 @@
     <t xml:space="preserve">الملفات</t>
   </si>
   <si>
-    <t xml:space="preserve">/public/files</t>
+    <t xml:space="preserve">/public/file</t>
   </si>
   <si>
     <t xml:space="preserve">FileList</t>
@@ -360,7 +360,7 @@
     <t xml:space="preserve">معارض الصور</t>
   </si>
   <si>
-    <t xml:space="preserve">/public/galleries</t>
+    <t xml:space="preserve">/public/gallery</t>
   </si>
   <si>
     <t xml:space="preserve">GalleryList</t>
@@ -381,7 +381,7 @@
     <t xml:space="preserve">translate</t>
   </si>
   <si>
-    <t xml:space="preserve">/public/translations</t>
+    <t xml:space="preserve">/public/translation</t>
   </si>
   <si>
     <t xml:space="preserve">TranslationList</t>
@@ -399,7 +399,7 @@
     <t xml:space="preserve">المدن</t>
   </si>
   <si>
-    <t xml:space="preserve">/property/cities</t>
+    <t xml:space="preserve">/property/city</t>
   </si>
   <si>
     <t xml:space="preserve">CityList</t>
@@ -420,7 +420,7 @@
     <t xml:space="preserve">map-pin-user-line</t>
   </si>
   <si>
-    <t xml:space="preserve">/property/locations</t>
+    <t xml:space="preserve">/property/location</t>
   </si>
   <si>
     <t xml:space="preserve">LocationList</t>
@@ -438,7 +438,7 @@
     <t xml:space="preserve">الصفحات</t>
   </si>
   <si>
-    <t xml:space="preserve">/tenant/pages</t>
+    <t xml:space="preserve">/tenant/page</t>
   </si>
   <si>
     <t xml:space="preserve">PageList</t>
@@ -459,7 +459,7 @@
     <t xml:space="preserve">grid-line</t>
   </si>
   <si>
-    <t xml:space="preserve">/tenant/sections</t>
+    <t xml:space="preserve">/tenant/section</t>
   </si>
   <si>
     <t xml:space="preserve">SectionList</t>
@@ -480,7 +480,7 @@
     <t xml:space="preserve">ball-pen-line</t>
   </si>
   <si>
-    <t xml:space="preserve">/tenant/partials</t>
+    <t xml:space="preserve">/tenant/partial</t>
   </si>
   <si>
     <t xml:space="preserve">PartialList</t>
@@ -492,6 +492,9 @@
     <t xml:space="preserve">01_c_cities</t>
   </si>
   <si>
+    <t xml:space="preserve">/property/citie</t>
+  </si>
+  <si>
     <t xml:space="preserve">02_c_locations</t>
   </si>
   <si>
@@ -525,6 +528,9 @@
     <t xml:space="preserve">user_password#</t>
   </si>
   <si>
+    <t xml:space="preserve">user_image</t>
+  </si>
+  <si>
     <t xml:space="preserve">ahmed</t>
   </si>
   <si>
@@ -540,10 +546,16 @@
     <t xml:space="preserve">super admin</t>
   </si>
   <si>
+    <t xml:space="preserve">images/avatar1.webp</t>
+  </si>
+  <si>
     <t xml:space="preserve">kareem</t>
   </si>
   <si>
     <t xml:space="preserve">kareem@devkit.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">images/avatar2.webp</t>
   </si>
 </sst>
 </file>
@@ -651,40 +663,44 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -957,63 +973,63 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="95.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="98.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="95.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="98.16"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1041,38 +1057,38 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="94.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="9.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="94.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="9.16"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1103,58 +1119,58 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="40.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6"/>
-      <c r="B3" s="0" t="s">
+      <c r="A3" s="7"/>
+      <c r="B3" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6"/>
+      <c r="A4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6"/>
+      <c r="A5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6"/>
+      <c r="A6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6"/>
+      <c r="A7" s="7"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6"/>
+      <c r="A8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6"/>
+      <c r="A9" s="7"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6"/>
+      <c r="A10" s="7"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6"/>
+      <c r="A11" s="7"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6"/>
+      <c r="A12" s="7"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:A12"/>
@@ -1182,240 +1198,240 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="149.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="9.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="149.33"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="17.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="17.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="G3" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="17.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="G4" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="17.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G5" s="0" t="s">
+      <c r="G5" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="17.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G6" s="0" t="s">
+      <c r="G6" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="17.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="7" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="G7" s="0" t="s">
+      <c r="G7" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="17.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+    <row r="8" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="0" t="s">
+      <c r="F8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G8" s="0" t="s">
+      <c r="G8" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="17.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+    <row r="9" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G9" s="0" t="s">
+      <c r="G9" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="17.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+    <row r="10" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E10" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="G10" s="0" t="s">
+      <c r="G10" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="17.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+    <row r="11" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G11" s="0" t="s">
+      <c r="G11" s="1" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1440,629 +1456,629 @@
   </sheetPr>
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E35" activeCellId="0" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="140.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="16.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="140.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="H2" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="G3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="H3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="I3" s="1" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="F4" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="G4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="0" t="s">
+      <c r="H4" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="I4" s="1" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="F5" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="G5" s="0" t="s">
+      <c r="G5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H5" s="0" t="s">
+      <c r="H5" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="I5" s="0" t="s">
+      <c r="I5" s="1" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="F6" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="G6" s="0" t="s">
+      <c r="G6" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H6" s="0" t="s">
+      <c r="H6" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="I6" s="0" t="s">
+      <c r="I6" s="1" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="F7" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="G7" s="0" t="s">
+      <c r="G7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H7" s="0" t="s">
+      <c r="H7" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="I7" s="0" t="s">
+      <c r="I7" s="1" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F8" s="0" t="s">
+      <c r="F8" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="G8" s="0" t="s">
+      <c r="G8" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H8" s="0" t="s">
+      <c r="H8" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="I8" s="0" t="s">
+      <c r="I8" s="1" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="F9" s="0" t="s">
+      <c r="F9" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="G9" s="0" t="s">
+      <c r="G9" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H9" s="0" t="s">
+      <c r="H9" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="I9" s="0" t="s">
+      <c r="I9" s="1" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E10" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F10" s="0" t="s">
+      <c r="F10" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="G10" s="0" t="s">
+      <c r="G10" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H10" s="0" t="s">
+      <c r="H10" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="I10" s="0" t="s">
+      <c r="I10" s="1" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="F11" s="0" t="s">
+      <c r="F11" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="G11" s="0" t="s">
+      <c r="G11" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H11" s="0" t="s">
+      <c r="H11" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="I11" s="0" t="s">
+      <c r="I11" s="1" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E12" s="0" t="s">
+      <c r="E12" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F12" s="0" t="s">
+      <c r="F12" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="G12" s="0" t="s">
+      <c r="G12" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="H12" s="0" t="s">
+      <c r="H12" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="I12" s="0" t="s">
+      <c r="I12" s="1" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E13" s="0" t="s">
+      <c r="E13" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="F13" s="0" t="s">
+      <c r="F13" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="G13" s="0" t="s">
+      <c r="G13" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="H13" s="0" t="s">
+      <c r="H13" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="I13" s="0" t="s">
+      <c r="I13" s="1" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="E14" s="0" t="s">
+      <c r="E14" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="F14" s="0" t="s">
+      <c r="F14" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="G14" s="0" t="s">
+      <c r="G14" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="H14" s="0" t="s">
+      <c r="H14" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="I14" s="0" t="s">
+      <c r="I14" s="1" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="E15" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F15" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="G15" s="0" t="s">
+      <c r="F15" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H15" s="0" t="s">
+      <c r="H15" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="I15" s="0" t="s">
+      <c r="I15" s="1" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="C16" s="0" t="s">
+      <c r="B16" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D16" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E16" s="0" t="s">
+      <c r="E16" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="F16" s="0" t="s">
+      <c r="F16" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="G16" s="0" t="s">
+      <c r="G16" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H16" s="0" t="s">
+      <c r="H16" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="I16" s="0" t="s">
+      <c r="I16" s="1" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="C17" s="0" t="s">
+      <c r="B17" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="D17" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E17" s="0" t="s">
+      <c r="E17" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F17" s="0" t="s">
+      <c r="F17" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="G17" s="0" t="s">
+      <c r="G17" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="H17" s="0" t="s">
+      <c r="H17" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="I17" s="0" t="s">
+      <c r="I17" s="1" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="C18" s="0" t="s">
+      <c r="B18" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="D18" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E18" s="0" t="s">
+      <c r="E18" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="F18" s="0" t="s">
+      <c r="F18" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="G18" s="0" t="s">
+      <c r="G18" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="H18" s="0" t="s">
+      <c r="H18" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="I18" s="0" t="s">
+      <c r="I18" s="1" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="C19" s="0" t="s">
+      <c r="B19" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="D19" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="E19" s="0" t="s">
+      <c r="E19" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="F19" s="0" t="s">
+      <c r="F19" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="G19" s="0" t="s">
+      <c r="G19" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="H19" s="0" t="s">
+      <c r="H19" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="I19" s="0" t="s">
+      <c r="I19" s="1" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="C20" s="0" t="s">
+      <c r="B20" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="D20" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E20" s="0" t="s">
+      <c r="E20" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="F20" s="0" t="s">
+      <c r="F20" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="G20" s="0" t="s">
+      <c r="G20" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="H20" s="0" t="s">
+      <c r="H20" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="I20" s="0" t="s">
+      <c r="I20" s="1" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="C21" s="0" t="s">
+      <c r="B21" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D21" s="0" t="s">
+      <c r="D21" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E21" s="0" t="s">
+      <c r="E21" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F21" s="0" t="s">
+      <c r="F21" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="G21" s="0" t="s">
+      <c r="G21" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="H21" s="0" t="s">
+      <c r="H21" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="I21" s="0" t="s">
+      <c r="I21" s="1" t="s">
         <v>106</v>
       </c>
     </row>
@@ -2085,84 +2101,93 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C28" activeCellId="0" sqref="C28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="58.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="34.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="58.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="34.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="94"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="E1" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>166</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="E2" s="7" t="n">
+      <c r="C2" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E2" s="8" t="n">
         <v>12345678</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>169</v>
+      <c r="F2" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>166</v>
-      </c>
-      <c r="C3" s="2" t="n">
+      <c r="A3" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C3" s="3" t="n">
         <v>1202290100</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E3" s="7" t="n">
+      <c r="D3" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="E3" s="8" t="n">
         <v>12345678</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="5" t="s">
         <v>17</v>
       </c>
+      <c r="G3" s="1" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F5" s="8"/>
+      <c r="F5" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>